<commit_message>
(to the second one) Added action.py, tiles.py, and npc.py. Hope to have trading in this game.
</commit_message>
<xml_diff>
--- a/the_second_one/map_folder/the_map.xlsx
+++ b/the_second_one/map_folder/the_map.xlsx
@@ -19,12 +19,87 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="27">
   <si>
     <t>start_room</t>
   </si>
   <si>
-    <t>hallway</t>
+    <t>seller_room</t>
+  </si>
+  <si>
+    <t>long_hallway</t>
+  </si>
+  <si>
+    <t>split_2_room</t>
+  </si>
+  <si>
+    <t>zombie_room</t>
+  </si>
+  <si>
+    <t>creepy_chamber_room</t>
+  </si>
+  <si>
+    <t>huge_floating_skull_bossroom</t>
+  </si>
+  <si>
+    <t>find_5_gold_room</t>
+  </si>
+  <si>
+    <t>random_person_room</t>
+  </si>
+  <si>
+    <t>find_10_gold_room</t>
+  </si>
+  <si>
+    <t>crazy_guy_room</t>
+  </si>
+  <si>
+    <t>split_3_room</t>
+  </si>
+  <si>
+    <t>tall_man_room</t>
+  </si>
+  <si>
+    <t>find_chalk_room</t>
+  </si>
+  <si>
+    <t>stitched_monster_room</t>
+  </si>
+  <si>
+    <t>find_eraser_room</t>
+  </si>
+  <si>
+    <t>sketchy_guy_room</t>
+  </si>
+  <si>
+    <t>huge_judge_bossroom</t>
+  </si>
+  <si>
+    <t>find_15_gold_room</t>
+  </si>
+  <si>
+    <t>find_slippers_room</t>
+  </si>
+  <si>
+    <t>atbash_room</t>
+  </si>
+  <si>
+    <t>base64_room</t>
+  </si>
+  <si>
+    <t>find_20_gold_room</t>
+  </si>
+  <si>
+    <t>caesarian_6_room</t>
+  </si>
+  <si>
+    <t>morse_room</t>
+  </si>
+  <si>
+    <t>little_boy_room</t>
+  </si>
+  <si>
+    <t>victory_room</t>
   </si>
 </sst>
 </file>
@@ -342,30 +417,266 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A6:B8"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.21875" customWidth="1"/>
+    <col min="2" max="2" width="13.21875" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" customWidth="1"/>
+    <col min="5" max="5" width="12.5546875" customWidth="1"/>
+    <col min="6" max="6" width="12.88671875" customWidth="1"/>
+    <col min="7" max="7" width="11.77734375" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" customWidth="1"/>
+    <col min="9" max="9" width="11.21875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>0</v>
-      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I6" t="s">
+        <v>3</v>
+      </c>
+      <c r="J6" t="s">
+        <v>2</v>
+      </c>
+      <c r="K6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" t="s">
+        <v>20</v>
+      </c>
+      <c r="K7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" t="s">
+        <v>19</v>
+      </c>
+      <c r="K8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I9" t="s">
+        <v>3</v>
+      </c>
+      <c r="J9" t="s">
+        <v>14</v>
+      </c>
+      <c r="K9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C20" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C21" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
(on the second one) The game currently works 9sort of)[D[D[D[D[D[D[D[D[D[([C[C[C[C[C[C[C[C[C[C[C[C[D[D[D[D. All that is left is to find out why the trade and heal commands do not show up.
</commit_message>
<xml_diff>
--- a/the_second_one/map_folder/the_map.xlsx
+++ b/the_second_one/map_folder/the_map.xlsx
@@ -19,14 +19,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="26">
   <si>
     <t>start_room</t>
   </si>
   <si>
-    <t>seller_room</t>
-  </si>
-  <si>
     <t>long_hallway</t>
   </si>
   <si>
@@ -57,9 +54,6 @@
     <t>split_3_room</t>
   </si>
   <si>
-    <t>tall_man_room</t>
-  </si>
-  <si>
     <t>find_chalk_room</t>
   </si>
   <si>
@@ -96,10 +90,13 @@
     <t>morse_room</t>
   </si>
   <si>
-    <t>little_boy_room</t>
-  </si>
-  <si>
     <t>victory_room</t>
+  </si>
+  <si>
+    <t>trader_room</t>
+  </si>
+  <si>
+    <t>little_boy_bossroom</t>
   </si>
 </sst>
 </file>
@@ -420,7 +417,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -441,222 +438,222 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" t="s">
         <v>15</v>
-      </c>
-      <c r="E4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H4" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="I7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="K7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
         <v>11</v>
       </c>
-      <c r="D8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" t="s">
-        <v>13</v>
-      </c>
       <c r="G8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="K8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="K9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F13" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C15" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C16" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="3:3" x14ac:dyDescent="0.3">
@@ -666,17 +663,17 @@
     </row>
     <row r="19" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C19" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C21" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>